<commit_message>
full design class works
</commit_message>
<xml_diff>
--- a/Second part/covidsim.xlsx
+++ b/Second part/covidsim.xlsx
@@ -432,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2678844.75</v>
+        <v>6352690.35</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2678838.450002352</v>
+        <v>6352689.550000126</v>
       </c>
       <c r="C3">
-        <v>6.299997648240852</v>
+        <v>0.799999874069122</v>
       </c>
       <c r="D3">
         <v>0.871134</v>
@@ -490,22 +490,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2678813.250250903</v>
+        <v>6352686.350002599</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>32.25862531718494</v>
+        <v>4.758871941207106</v>
       </c>
       <c r="E4">
-        <v>0.1928990238183441</v>
+        <v>0.192900367228444</v>
       </c>
       <c r="F4">
-        <v>0.04822475595458604</v>
+        <v>0.048225091807111</v>
       </c>
       <c r="G4">
-        <v>7.299997648224235</v>
+        <v>1.799999874085188</v>
       </c>
       <c r="H4">
         <v>0.01675258</v>
@@ -519,25 +519,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2678610.023376983</v>
+        <v>6352682.542908044</v>
       </c>
       <c r="C5">
-        <v>203.2268739204904</v>
+        <v>3.807094556522632</v>
       </c>
       <c r="D5">
-        <v>28.10158530706058</v>
+        <v>4.145615149631512</v>
       </c>
       <c r="E5">
-        <v>3.518531031917828</v>
+        <v>0.6835058004889202</v>
       </c>
       <c r="F5">
-        <v>0.8796327579794569</v>
+        <v>0.17087645012223</v>
       </c>
       <c r="G5">
-        <v>32.49974909704179</v>
+        <v>4.999997400678694</v>
       </c>
       <c r="H5">
-        <v>0.03134609137048092</v>
+        <v>0.03134630967462215</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -548,25 +548,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2677797.364738652</v>
+        <v>6352667.314574885</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1040.367661820587</v>
+        <v>22.64681662547201</v>
       </c>
       <c r="E6">
-        <v>6.414079622481377</v>
+        <v>1.110886790970173</v>
       </c>
       <c r="F6">
-        <v>1.603519905620344</v>
+        <v>0.2777216977425432</v>
       </c>
       <c r="G6">
-        <v>235.7266230173409</v>
+        <v>8.807091956026852</v>
       </c>
       <c r="H6">
-        <v>0.571761292686647</v>
+        <v>0.1110696925794495</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -577,25 +577,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2671245.613547285</v>
+        <v>6352649.197190133</v>
       </c>
       <c r="C7">
-        <v>6551.751191366514</v>
+        <v>18.11738475294345</v>
       </c>
       <c r="D7">
-        <v>906.2996427124148</v>
+        <v>19.72841195421394</v>
       </c>
       <c r="E7">
-        <v>113.6684949090188</v>
+        <v>3.445610527976635</v>
       </c>
       <c r="F7">
-        <v>28.41712372725469</v>
+        <v>0.8614026319941587</v>
       </c>
       <c r="G7">
-        <v>1048.385261348449</v>
+        <v>24.03542511444539</v>
       </c>
       <c r="H7">
-        <v>1.042287938653224</v>
+        <v>0.1805191035326531</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -606,25 +606,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2645295.522835042</v>
+        <v>6352576.72867392</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>33293.31764562563</v>
+        <v>107.7720525026427</v>
       </c>
       <c r="E8">
-        <v>205.5276154658907</v>
+        <v>5.479418861440471</v>
       </c>
       <c r="F8">
-        <v>51.38190386647268</v>
+        <v>1.369854715360118</v>
       </c>
       <c r="G8">
-        <v>7600.136452714913</v>
+        <v>42.15280986670405</v>
       </c>
       <c r="H8">
-        <v>18.47113042271555</v>
+        <v>0.5599117107962032</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -635,25 +635,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2438174.532803317</v>
+        <v>6352490.512587539</v>
       </c>
       <c r="C9">
-        <v>207120.9900317253</v>
+        <v>86.21608638105322</v>
       </c>
       <c r="D9">
-        <v>29002.94097390444</v>
+        <v>93.88389918483716</v>
       </c>
       <c r="E9">
-        <v>3637.828952842845</v>
+        <v>16.58994151568492</v>
       </c>
       <c r="F9">
-        <v>909.4572382107112</v>
+        <v>4.147485378921229</v>
       </c>
       <c r="G9">
-        <v>33550.22716495767</v>
+        <v>114.6213260795921</v>
       </c>
       <c r="H9">
-        <v>33.39823751320724</v>
+        <v>0.8904055649840765</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -664,25 +664,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1821593.798410963</v>
+        <v>6352145.671413617</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>850609.1898334008</v>
+        <v>512.8441112129887</v>
       </c>
       <c r="E10">
-        <v>5314.20940450875</v>
+        <v>26.26758013553027</v>
       </c>
       <c r="F10">
-        <v>1328.552351127187</v>
+        <v>6.566895033882568</v>
       </c>
       <c r="G10">
-        <v>240671.2171966834</v>
+        <v>200.8374124607071</v>
       </c>
       <c r="H10">
-        <v>591.1472048369624</v>
+        <v>2.695865496298799</v>
       </c>
       <c r="I10">
         <v>8</v>
@@ -693,25 +693,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>6351735.431366157</v>
       </c>
       <c r="C11">
-        <v>2168662.685807084</v>
+        <v>410.2400474597652</v>
       </c>
       <c r="D11">
-        <v>440993.9081771816</v>
+        <v>446.7559419774156</v>
       </c>
       <c r="E11">
-        <v>55351.32481258787</v>
+        <v>79.13811552398866</v>
       </c>
       <c r="F11">
-        <v>13837.83120314697</v>
+        <v>19.78452888099716</v>
       </c>
       <c r="G11">
-        <v>857251.9515890365</v>
+        <v>545.6785863824189</v>
       </c>
       <c r="H11">
-        <v>863.5590282326718</v>
+        <v>4.268481772023669</v>
       </c>
       <c r="I11">
         <v>9</v>
@@ -722,25 +722,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>6350094.995789276</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2649111.867937323</v>
+        <v>2439.891529565515</v>
       </c>
       <c r="E12">
-        <v>23787.10565014157</v>
+        <v>125.1701449269209</v>
       </c>
       <c r="F12">
-        <v>5946.776412535393</v>
+        <v>31.29253623173022</v>
       </c>
       <c r="G12">
-        <v>2678845.75</v>
+        <v>955.9186338428408</v>
       </c>
       <c r="H12">
-        <v>8994.59028204553</v>
+        <v>12.85994377264816</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -751,25 +751,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>6348143.880315402</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1951.115473873935</v>
       </c>
       <c r="D13">
-        <v>2307731.417963712</v>
+        <v>2125.472467716525</v>
       </c>
       <c r="E13">
-        <v>296891.4656290305</v>
+        <v>376.7053944061126</v>
       </c>
       <c r="F13">
-        <v>74222.86640725764</v>
+        <v>94.17634860152816</v>
       </c>
       <c r="G13">
-        <v>2678845.75</v>
+        <v>2596.354210724123</v>
       </c>
       <c r="H13">
-        <v>3865.404668148006</v>
+        <v>20.34014855062464</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -780,25 +780,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>6340351.277937627</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2010343.3010564</v>
+        <v>11596.00427620061</v>
       </c>
       <c r="E14">
-        <v>534801.9591548798</v>
+        <v>595.254228937092</v>
       </c>
       <c r="F14">
-        <v>133700.4897887199</v>
+        <v>148.813557234273</v>
       </c>
       <c r="G14">
-        <v>2678845.75</v>
+        <v>4547.469684598036</v>
       </c>
       <c r="H14">
-        <v>48244.86316471746</v>
+        <v>61.2146265909933</v>
       </c>
       <c r="I14">
         <v>12</v>
@@ -809,25 +809,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>6331092.494662211</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>9258.783275416487</v>
       </c>
       <c r="D15">
-        <v>1751278.401222466</v>
+        <v>10101.67358914374</v>
       </c>
       <c r="E15">
-        <v>742053.8790220272</v>
+        <v>1790.718778582586</v>
       </c>
       <c r="F15">
-        <v>185513.4697555068</v>
+        <v>447.6796946456465</v>
       </c>
       <c r="G15">
-        <v>2678845.75</v>
+        <v>12340.07206237223</v>
       </c>
       <c r="H15">
-        <v>86905.31836266797</v>
+        <v>96.72881220227745</v>
       </c>
       <c r="I15">
         <v>13</v>
@@ -838,25 +838,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>6294323.637750985</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1525598.158770532</v>
+        <v>54843.62853917486</v>
       </c>
       <c r="E16">
-        <v>922598.0729835747</v>
+        <v>2819.266967871285</v>
       </c>
       <c r="F16">
-        <v>230649.5182458937</v>
+        <v>704.8167419678211</v>
       </c>
       <c r="G16">
-        <v>2678845.75</v>
+        <v>21598.85533778835</v>
       </c>
       <c r="H16">
-        <v>120583.7553410794</v>
+        <v>290.9918015196703</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -867,25 +867,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>6250851.851892015</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>43471.78585896989</v>
       </c>
       <c r="D17">
-        <v>1329000.426442408</v>
+        <v>47776.14950384555</v>
       </c>
       <c r="E17">
-        <v>1079876.258846073</v>
+        <v>8473.250196134732</v>
       </c>
       <c r="F17">
-        <v>269969.0647115184</v>
+        <v>2118.312549033683</v>
       </c>
       <c r="G17">
-        <v>2678845.75</v>
+        <v>58367.71224901453</v>
       </c>
       <c r="H17">
-        <v>149922.1868598309</v>
+        <v>458.1308822790838</v>
       </c>
       <c r="I17">
         <v>15</v>
@@ -896,25 +896,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>6082755.416822709</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1157737.457488481</v>
+        <v>253539.3903816155</v>
       </c>
       <c r="E18">
-        <v>1216886.634009215</v>
+        <v>13117.23423654065</v>
       </c>
       <c r="F18">
-        <v>304221.6585023038</v>
+        <v>3279.308559135163</v>
       </c>
       <c r="G18">
-        <v>2678845.75</v>
+        <v>101839.4981079847</v>
       </c>
       <c r="H18">
-        <v>175479.8920624869</v>
+        <v>1376.903156871894</v>
       </c>
       <c r="I18">
         <v>16</v>
@@ -925,25 +925,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>5888542.537240993</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>194212.8795817161</v>
       </c>
       <c r="D19">
-        <v>1008544.46229177</v>
+        <v>220866.7833006982</v>
       </c>
       <c r="E19">
-        <v>1336241.030166584</v>
+        <v>39255.31990127447</v>
       </c>
       <c r="F19">
-        <v>334060.257541646</v>
+        <v>9813.829975318617</v>
       </c>
       <c r="G19">
-        <v>2678845.75</v>
+        <v>269935.9331772905</v>
       </c>
       <c r="H19">
-        <v>197744.0780264975</v>
+        <v>2131.550563437856</v>
       </c>
       <c r="I19">
         <v>17</v>
@@ -954,25 +954,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>5220913.494530735</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>878577.3716140791</v>
+        <v>1061070.149690331</v>
       </c>
       <c r="E20">
-        <v>1440214.702708737</v>
+        <v>56566.16462314687</v>
       </c>
       <c r="F20">
-        <v>360053.6756771842</v>
+        <v>14141.54115578672</v>
       </c>
       <c r="G20">
-        <v>2678845.75</v>
+        <v>464148.8127590064</v>
       </c>
       <c r="H20">
-        <v>217139.1674020699</v>
+        <v>6378.989483957101</v>
       </c>
       <c r="I20">
         <v>18</v>
@@ -983,25 +983,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>4523287.224598764</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>697626.2699319711</v>
       </c>
       <c r="D21">
-        <v>765358.620043659</v>
+        <v>924334.2837803368</v>
       </c>
       <c r="E21">
-        <v>1530789.703965073</v>
+        <v>165954.8573511423</v>
       </c>
       <c r="F21">
-        <v>382697.4259912682</v>
+        <v>41488.71433778557</v>
       </c>
       <c r="G21">
-        <v>2678845.75</v>
+        <v>1131777.855469265</v>
       </c>
       <c r="H21">
-        <v>234034.8891901698</v>
+        <v>9192.001751261367</v>
       </c>
       <c r="I21">
         <v>19</v>
@@ -1012,25 +1012,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>2946637.994522575</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>666729.9161131128</v>
+        <v>3165296.067568534</v>
       </c>
       <c r="E22">
-        <v>1609692.66710951</v>
+        <v>192605.8303271122</v>
       </c>
       <c r="F22">
-        <v>402423.1667773774</v>
+        <v>48151.45758177806</v>
       </c>
       <c r="G22">
-        <v>2678845.75</v>
+        <v>1829404.125401235</v>
       </c>
       <c r="H22">
-        <v>248753.3268943243</v>
+        <v>26967.66431956062</v>
       </c>
       <c r="I22">
         <v>20</v>
@@ -1041,25 +1041,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1772083.004488584</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1174554.990033991</v>
       </c>
       <c r="D23">
-        <v>580811.0987432804</v>
+        <v>2757397.024525247</v>
       </c>
       <c r="E23">
-        <v>1678427.721005376</v>
+        <v>518925.0647617415</v>
       </c>
       <c r="F23">
-        <v>419606.9302513439</v>
+        <v>129731.2661904354</v>
       </c>
       <c r="G23">
-        <v>2678845.75</v>
+        <v>3406053.355477424</v>
       </c>
       <c r="H23">
-        <v>261575.0584052953</v>
+        <v>31298.44742815574</v>
       </c>
       <c r="I23">
         <v>21</v>
@@ -1070,25 +1070,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>704171.0970232752</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>505964.2956926289</v>
+        <v>5037337.070538723</v>
       </c>
       <c r="E24">
-        <v>1738305.163445897</v>
+        <v>488946.5459504012</v>
       </c>
       <c r="F24">
-        <v>434576.2908614743</v>
+        <v>122236.6364876003</v>
       </c>
       <c r="G24">
-        <v>2678845.75</v>
+        <v>4580608.345511416</v>
       </c>
       <c r="H24">
-        <v>272744.5046633736</v>
+        <v>84325.323023783</v>
       </c>
       <c r="I24">
         <v>22</v>
@@ -1099,25 +1099,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>257475.7390267292</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>446695.357996546</v>
       </c>
       <c r="D25">
-        <v>440762.7007639025</v>
+        <v>4388195.59160668</v>
       </c>
       <c r="E25">
-        <v>1790466.439388878</v>
+        <v>1008259.729096036</v>
       </c>
       <c r="F25">
-        <v>447616.6098472195</v>
+        <v>252064.9322740089</v>
       </c>
       <c r="G25">
-        <v>2678845.75</v>
+        <v>5648520.252976725</v>
       </c>
       <c r="H25">
-        <v>282474.5890599583</v>
+        <v>79453.81371694019</v>
       </c>
       <c r="I25">
         <v>23</v>
@@ -1128,25 +1128,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>91504.74641211731</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>383963.3745672614</v>
+        <v>4810823.033388617</v>
       </c>
       <c r="E26">
-        <v>1835905.900346191</v>
+        <v>1160290.856159413</v>
       </c>
       <c r="F26">
-        <v>458976.4750865478</v>
+        <v>290072.7140398532</v>
       </c>
       <c r="G26">
-        <v>2678845.75</v>
+        <v>6095215.610973271</v>
       </c>
       <c r="H26">
-        <v>290950.7964006927</v>
+        <v>163842.2059781058</v>
       </c>
       <c r="I26">
         <v>24</v>
@@ -1157,25 +1157,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>36068.31892645982</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>55436.42748565751</v>
       </c>
       <c r="D27">
-        <v>334483.5503402767</v>
+        <v>4190871.51236796</v>
       </c>
       <c r="E27">
-        <v>1875489.759727779</v>
+        <v>1656252.072975939</v>
       </c>
       <c r="F27">
-        <v>468872.4399319447</v>
+        <v>414063.0182439848</v>
       </c>
       <c r="G27">
-        <v>2678845.75</v>
+        <v>6261186.603587883</v>
       </c>
       <c r="H27">
-        <v>298334.7088062561</v>
+        <v>188547.2641259046</v>
       </c>
       <c r="I27">
         <v>25</v>
@@ -1186,25 +1186,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>16506.1961687579</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>291379.9931421266</v>
+        <v>3806528.915536088</v>
       </c>
       <c r="E28">
-        <v>1909972.605486299</v>
+        <v>2023724.990636123</v>
       </c>
       <c r="F28">
-        <v>477493.1513715747</v>
+        <v>505931.2476590307</v>
       </c>
       <c r="G28">
-        <v>2678845.75</v>
+        <v>6316623.03107354</v>
       </c>
       <c r="H28">
-        <v>304767.0859557641</v>
+        <v>269140.9618585901</v>
       </c>
       <c r="I28">
         <v>26</v>
@@ -1215,25 +1215,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>8593.79375029153</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>7912.402418466364</v>
       </c>
       <c r="D29">
-        <v>253831.0189458732</v>
+        <v>3315996.760306615</v>
       </c>
       <c r="E29">
-        <v>1940011.784843301</v>
+        <v>2416150.714819701</v>
       </c>
       <c r="F29">
-        <v>485002.9462108253</v>
+        <v>604037.6787049253</v>
       </c>
       <c r="G29">
-        <v>2678845.75</v>
+        <v>6336185.153831242</v>
       </c>
       <c r="H29">
-        <v>310370.5483915236</v>
+        <v>328855.31097837</v>
       </c>
       <c r="I29">
         <v>27</v>
@@ -1244,25 +1244,25 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>4983.131125689103</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>221120.8308583943</v>
+        <v>2915361.866201557</v>
       </c>
       <c r="E30">
-        <v>1966179.935313284</v>
+        <v>2745877.082138203</v>
       </c>
       <c r="F30">
-        <v>491544.9838283211</v>
+        <v>686469.2705345507</v>
       </c>
       <c r="G30">
-        <v>2678845.75</v>
+        <v>6344097.556249708</v>
       </c>
       <c r="H30">
-        <v>315251.9150370365</v>
+        <v>392624.4911582015</v>
       </c>
       <c r="I30">
         <v>28</v>
@@ -1273,25 +1273,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>3153.653865394874</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1829.477260294228</v>
       </c>
       <c r="D31">
-        <v>192625.8738689965</v>
+        <v>2539670.843951627</v>
       </c>
       <c r="E31">
-        <v>1988975.900904803</v>
+        <v>3046429.899938147</v>
       </c>
       <c r="F31">
-        <v>497243.9752262008</v>
+        <v>761607.4749845368</v>
       </c>
       <c r="G31">
-        <v>2678845.75</v>
+        <v>6347708.21887431</v>
       </c>
       <c r="H31">
-        <v>319504.2394884087</v>
+        <v>446205.0258474579</v>
       </c>
       <c r="I31">
         <v>29</v>
@@ -1302,25 +1302,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>2142.914612950391</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>167802.9480069944</v>
+        <v>2219336.830054891</v>
       </c>
       <c r="E32">
-        <v>2008834.241594405</v>
+        <v>3304969.284265726</v>
       </c>
       <c r="F32">
-        <v>502208.5603986012</v>
+        <v>826242.3210664315</v>
       </c>
       <c r="G32">
-        <v>2678845.75</v>
+        <v>6349537.696134605</v>
       </c>
       <c r="H32">
-        <v>323208.5838970305</v>
+        <v>495044.8587399489</v>
       </c>
       <c r="I32">
         <v>30</v>
@@ -1331,25 +1331,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1544.006331447481</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>598.90828150291</v>
       </c>
       <c r="D33">
-        <v>146178.853309125</v>
+        <v>1933339.770113038</v>
       </c>
       <c r="E33">
-        <v>2026133.5173527</v>
+        <v>3533766.93221921</v>
       </c>
       <c r="F33">
-        <v>506533.3793381751</v>
+        <v>883441.7330548024</v>
       </c>
       <c r="G33">
-        <v>2678845.75</v>
+        <v>6350548.435387049</v>
       </c>
       <c r="H33">
-        <v>326435.5642590908</v>
+        <v>537057.5086931805</v>
       </c>
       <c r="I33">
         <v>31</v>
@@ -1360,25 +1360,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1167.720217284553</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>127341.3691985913</v>
+        <v>1686656.308178567</v>
       </c>
       <c r="E34">
-        <v>2041203.504641127</v>
+        <v>3731893.857283318</v>
       </c>
       <c r="F34">
-        <v>510300.8761602818</v>
+        <v>932973.4643208296</v>
       </c>
       <c r="G34">
-        <v>2678845.75</v>
+        <v>6351147.343668552</v>
       </c>
       <c r="H34">
-        <v>329246.6965698138</v>
+        <v>574237.1264856216</v>
       </c>
       <c r="I34">
         <v>32</v>
@@ -1389,25 +1389,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>919.6939793127506</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>248.0262379718025</v>
       </c>
       <c r="D35">
-        <v>110931.3963154456</v>
+        <v>1469303.656368828</v>
       </c>
       <c r="E35">
-        <v>2054331.482947643</v>
+        <v>3905775.97873111</v>
       </c>
       <c r="F35">
-        <v>513582.8707369108</v>
+        <v>976443.9946827774</v>
       </c>
       <c r="G35">
-        <v>2678845.75</v>
+        <v>6351523.629782715</v>
       </c>
       <c r="H35">
-        <v>331695.5695041831</v>
+        <v>606432.7518085393</v>
       </c>
       <c r="I35">
         <v>33</v>
@@ -1418,25 +1418,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>749.4253955970053</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>96636.11099785942</v>
+        <v>1281034.757838621</v>
       </c>
       <c r="E36">
-        <v>2065767.711201712</v>
+        <v>4056725.733412626</v>
       </c>
       <c r="F36">
-        <v>516441.9278004281</v>
+        <v>1014181.433353156</v>
       </c>
       <c r="G36">
-        <v>2678845.75</v>
+        <v>6351771.656020687</v>
       </c>
       <c r="H36">
-        <v>333828.8659789921</v>
+        <v>634688.5965438053</v>
       </c>
       <c r="I36">
         <v>34</v>
@@ -1447,25 +1447,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>628.5267178840736</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>120.8986777129315</v>
       </c>
       <c r="D37">
-        <v>84183.00191800926</v>
+        <v>1115952.932734989</v>
       </c>
       <c r="E37">
-        <v>2075730.198465592</v>
+        <v>4188791.19349553</v>
       </c>
       <c r="F37">
-        <v>518932.5496163981</v>
+        <v>1047197.798373883</v>
       </c>
       <c r="G37">
-        <v>2678845.75</v>
+        <v>6351941.924604403</v>
       </c>
       <c r="H37">
-        <v>335687.2530702783</v>
+        <v>659217.9316795517</v>
       </c>
       <c r="I37">
         <v>35</v>
@@ -1476,25 +1476,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>540.1644057550124</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>73334.67519284307</v>
+        <v>972688.5145767028</v>
       </c>
       <c r="E38">
-        <v>2084408.859845726</v>
+        <v>4303570.136814034</v>
       </c>
       <c r="F38">
-        <v>521102.2149614314</v>
+        <v>1075892.534203508</v>
       </c>
       <c r="G38">
-        <v>2678845.75</v>
+        <v>6352062.823282115</v>
       </c>
       <c r="H38">
-        <v>337306.1572506588</v>
+        <v>680678.5689430237</v>
       </c>
       <c r="I38">
         <v>36</v>
@@ -1505,25 +1505,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>473.9988473151489</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>66.1655584398635</v>
       </c>
       <c r="D39">
-        <v>63884.32893944216</v>
+        <v>847342.0364572614</v>
       </c>
       <c r="E39">
-        <v>2091969.136848446</v>
+        <v>4403847.319309587</v>
       </c>
       <c r="F39">
-        <v>522992.2842121116</v>
+        <v>1100961.829827397</v>
       </c>
       <c r="G39">
-        <v>2678845.75</v>
+        <v>6352151.185594245</v>
       </c>
       <c r="H39">
-        <v>338716.4397249304</v>
+        <v>699330.1472322805</v>
       </c>
       <c r="I39">
         <v>37</v>
@@ -1534,25 +1534,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>423.4058080308445</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>55651.81100633201</v>
+        <v>738454.3997259369</v>
       </c>
       <c r="E40">
-        <v>2098555.151194935</v>
+        <v>4491050.835572827</v>
       </c>
       <c r="F40">
-        <v>524638.7877987337</v>
+        <v>1122762.708893207</v>
       </c>
       <c r="G40">
-        <v>2678845.75</v>
+        <v>6352217.351152685</v>
       </c>
       <c r="H40">
-        <v>339944.9847378726</v>
+        <v>715625.1893878079</v>
       </c>
       <c r="I40">
         <v>38</v>
@@ -1563,25 +1563,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>384.0315189827995</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>39.3742890480448</v>
       </c>
       <c r="D41">
-        <v>48480.18472919</v>
+        <v>643292.7350508542</v>
       </c>
       <c r="E41">
-        <v>2104292.452216648</v>
+        <v>4567180.167312892</v>
       </c>
       <c r="F41">
-        <v>526073.1130541619</v>
+        <v>1141795.041828223</v>
       </c>
       <c r="G41">
-        <v>2678845.75</v>
+        <v>6352267.944191969</v>
       </c>
       <c r="H41">
-        <v>341015.2120691769</v>
+        <v>729795.7607805844</v>
       </c>
       <c r="I41">
         <v>39</v>
@@ -1592,25 +1592,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>352.913943508613</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>42232.73724387821</v>
+        <v>560579.8921810609</v>
       </c>
       <c r="E42">
-        <v>2109290.410204898</v>
+        <v>4633406.835100344</v>
       </c>
       <c r="F42">
-        <v>527322.6025512244</v>
+        <v>1158351.708775086</v>
       </c>
       <c r="G42">
-        <v>2678845.75</v>
+        <v>6352307.318481017</v>
       </c>
       <c r="H42">
-        <v>341947.5234852053</v>
+        <v>742166.777188345</v>
       </c>
       <c r="I42">
         <v>40</v>
@@ -1621,25 +1621,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>328.0002243302051</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>24.91371917840791</v>
       </c>
       <c r="D43">
-        <v>36790.3733262086</v>
+        <v>488340.2037952563</v>
       </c>
       <c r="E43">
-        <v>2113644.301339033</v>
+        <v>4691198.585808988</v>
       </c>
       <c r="F43">
-        <v>528411.0753347583</v>
+        <v>1172799.646452247</v>
       </c>
       <c r="G43">
-        <v>2678845.75</v>
+        <v>6352338.436056491</v>
       </c>
       <c r="H43">
-        <v>342759.6916582959</v>
+        <v>752928.610703806</v>
       </c>
       <c r="I43">
         <v>41</v>
@@ -1650,25 +1650,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>307.8253067743839</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>32049.3450771534</v>
+        <v>425528.9995412677</v>
       </c>
       <c r="E44">
-        <v>2117437.123938277</v>
+        <v>4741483.620121566</v>
       </c>
       <c r="F44">
-        <v>529359.2809845693</v>
+        <v>1185370.905030391</v>
       </c>
       <c r="G44">
-        <v>2678845.75</v>
+        <v>6352363.349775669</v>
       </c>
       <c r="H44">
-        <v>343467.1989675929</v>
+        <v>762319.7701939605</v>
       </c>
       <c r="I44">
         <v>42</v>
@@ -1679,25 +1679,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>291.3297980070408</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>16.49550876734314</v>
       </c>
       <c r="D45">
-        <v>27919.27417444095</v>
+        <v>370692.7794863827</v>
       </c>
       <c r="E45">
-        <v>2120741.180660447</v>
+        <v>4785352.596165474</v>
       </c>
       <c r="F45">
-        <v>530185.2951651118</v>
+        <v>1196338.149041368</v>
       </c>
       <c r="G45">
-        <v>2678845.75</v>
+        <v>6352383.524693226</v>
       </c>
       <c r="H45">
-        <v>344083.5326399701</v>
+        <v>770491.0882697544</v>
       </c>
       <c r="I45">
         <v>43</v>
@@ -1708,25 +1708,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>277.7277472687484</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>24321.42898867745</v>
+        <v>323002.8979296609</v>
       </c>
       <c r="E46">
-        <v>2123619.456809058</v>
+        <v>4823528.579458456</v>
       </c>
       <c r="F46">
-        <v>530904.8642022645</v>
+        <v>1205882.144864614</v>
       </c>
       <c r="G46">
-        <v>2678845.75</v>
+        <v>6352400.020201992</v>
       </c>
       <c r="H46">
-        <v>344620.4418573226</v>
+        <v>777619.7968768895</v>
       </c>
       <c r="I46">
         <v>44</v>
@@ -1737,25 +1737,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>266.4308827102923</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>11.29686455845612</v>
       </c>
       <c r="D47">
-        <v>21187.22372062254</v>
+        <v>281378.8064850573</v>
       </c>
       <c r="E47">
-        <v>2126126.821023502</v>
+        <v>4856827.852614139</v>
       </c>
       <c r="F47">
-        <v>531531.7052558755</v>
+        <v>1214206.963153535</v>
       </c>
       <c r="G47">
-        <v>2678845.75</v>
+        <v>6352413.622252731</v>
       </c>
       <c r="H47">
-        <v>345088.1617314719</v>
+        <v>783823.3941619991</v>
       </c>
       <c r="I47">
         <v>45</v>
@@ -1766,25 +1766,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>256.9886500856697</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>18456.91094864079</v>
+        <v>245173.7499356657</v>
       </c>
       <c r="E48">
-        <v>2128311.071241087</v>
+        <v>4885808.489131398</v>
       </c>
       <c r="F48">
-        <v>532077.7678102718</v>
+        <v>1221452.12228285</v>
       </c>
       <c r="G48">
-        <v>2678845.75</v>
+        <v>6352424.91911729</v>
       </c>
       <c r="H48">
-        <v>345495.6084163191</v>
+        <v>789234.5260497977</v>
       </c>
       <c r="I48">
         <v>46</v>
@@ -1795,25 +1795,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>249.0541394902625</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>7.934510595407194</v>
       </c>
       <c r="D49">
-        <v>16078.44266233325</v>
+        <v>213579.1894764563</v>
       </c>
       <c r="E49">
-        <v>2130213.845870133</v>
+        <v>4911084.137498766</v>
       </c>
       <c r="F49">
-        <v>532553.4614675334</v>
+        <v>1227771.034374692</v>
       </c>
       <c r="G49">
-        <v>2678845.75</v>
+        <v>6352434.361349914</v>
       </c>
       <c r="H49">
-        <v>345850.5490766767</v>
+        <v>793943.8794838523</v>
       </c>
       <c r="I49">
         <v>47</v>
@@ -1824,25 +1824,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>242.3545705873175</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>14006.47807020901</v>
+        <v>186095.0326961245</v>
       </c>
       <c r="E50">
-        <v>2131871.417543833</v>
+        <v>4933083.17018663</v>
       </c>
       <c r="F50">
-        <v>532967.8543859583</v>
+        <v>1233270.792546658</v>
       </c>
       <c r="G50">
-        <v>2678845.75</v>
+        <v>6352442.295860509</v>
       </c>
       <c r="H50">
-        <v>346159.7499538967</v>
+        <v>798051.1723435496</v>
       </c>
       <c r="I50">
         <v>48</v>
@@ -1853,25 +1853,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>236.6749643539687</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>5.679606233348904</v>
       </c>
       <c r="D51">
-        <v>12201.51926721346</v>
+        <v>162113.7102127057</v>
       </c>
       <c r="E51">
-        <v>2133315.384586229</v>
+        <v>4952268.228173366</v>
       </c>
       <c r="F51">
-        <v>533328.8461465572</v>
+        <v>1238067.057043341</v>
       </c>
       <c r="G51">
-        <v>2678845.75</v>
+        <v>6352448.995429412</v>
       </c>
       <c r="H51">
-        <v>346429.1053508729</v>
+        <v>801626.0151553275</v>
       </c>
       <c r="I51">
         <v>49</v>
@@ -1882,25 +1882,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>231.8425633336233</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>10629.15828532473</v>
+        <v>141250.7651570821</v>
       </c>
       <c r="E52">
-        <v>2134573.27337174</v>
+        <v>4968966.993823667</v>
       </c>
       <c r="F52">
-        <v>533643.3183429351</v>
+        <v>1242241.748455917</v>
       </c>
       <c r="G52">
-        <v>2678845.75</v>
+        <v>6352454.675035645</v>
       </c>
       <c r="H52">
-        <v>346663.7499952622</v>
+        <v>804743.587078172</v>
       </c>
       <c r="I52">
         <v>50</v>

</xml_diff>

<commit_message>
Added script for validation
</commit_message>
<xml_diff>
--- a/Second part/covidsim.xlsx
+++ b/Second part/covidsim.xlsx
@@ -432,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6352690.35</v>
+        <v>2678844.75</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6352689.550000126</v>
+        <v>2678838.450002352</v>
       </c>
       <c r="C3">
-        <v>0.799999874069122</v>
+        <v>6.299997648240852</v>
       </c>
       <c r="D3">
         <v>0.871134</v>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.07938145600000002</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -490,25 +490,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6352686.350002599</v>
+        <v>2678813.250250903</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>4.758871941207106</v>
+        <v>32.25862531718494</v>
       </c>
       <c r="E4">
-        <v>0.192900367228444</v>
+        <v>0.1928990238183441</v>
       </c>
       <c r="F4">
-        <v>0.048225091807111</v>
+        <v>0.04822475595458604</v>
       </c>
       <c r="G4">
-        <v>1.799999874085188</v>
+        <v>7.299997648224235</v>
       </c>
       <c r="H4">
-        <v>0.01675258</v>
+        <v>0.148533341291104</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -519,25 +519,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6352682.542908044</v>
+        <v>2678610.023376983</v>
       </c>
       <c r="C5">
-        <v>3.807094556522632</v>
+        <v>203.2268739204904</v>
       </c>
       <c r="D5">
-        <v>4.145615149631512</v>
+        <v>28.10158530706058</v>
       </c>
       <c r="E5">
-        <v>0.6835058004889202</v>
+        <v>3.518531031917828</v>
       </c>
       <c r="F5">
-        <v>0.17087645012223</v>
+        <v>0.8796327579794569</v>
       </c>
       <c r="G5">
-        <v>4.999997400678694</v>
+        <v>32.49974909704179</v>
       </c>
       <c r="H5">
-        <v>0.03134630967462215</v>
+        <v>2.709268894576728</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -548,25 +548,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6352667.314574885</v>
+        <v>2677797.364738652</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>22.64681662547201</v>
+        <v>1040.367661820587</v>
       </c>
       <c r="E6">
-        <v>1.110886790970173</v>
+        <v>6.414079622481377</v>
       </c>
       <c r="F6">
-        <v>0.2777216977425432</v>
+        <v>1.603519905620344</v>
       </c>
       <c r="G6">
-        <v>8.807091956026852</v>
+        <v>235.7266230173409</v>
       </c>
       <c r="H6">
-        <v>0.1110696925794495</v>
+        <v>4.940013652159404</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -577,25 +577,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>6352649.197190133</v>
+        <v>2671245.613547285</v>
       </c>
       <c r="C7">
-        <v>18.11738475294345</v>
+        <v>6551.751191366514</v>
       </c>
       <c r="D7">
-        <v>19.72841195421394</v>
+        <v>906.2996427124148</v>
       </c>
       <c r="E7">
-        <v>3.445610527976635</v>
+        <v>113.6684949090188</v>
       </c>
       <c r="F7">
-        <v>0.8614026319941587</v>
+        <v>28.41712372725469</v>
       </c>
       <c r="G7">
-        <v>24.03542511444539</v>
+        <v>1048.385261348449</v>
       </c>
       <c r="H7">
-        <v>0.1805191035326531</v>
+        <v>87.52474107994445</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -606,25 +606,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>6352576.72867392</v>
+        <v>2645295.522835042</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>107.7720525026427</v>
+        <v>33293.31764562563</v>
       </c>
       <c r="E8">
-        <v>5.479418861440471</v>
+        <v>205.5276154658907</v>
       </c>
       <c r="F8">
-        <v>1.369854715360118</v>
+        <v>51.38190386647268</v>
       </c>
       <c r="G8">
-        <v>42.15280986670405</v>
+        <v>7600.136452714913</v>
       </c>
       <c r="H8">
-        <v>0.5599117107962032</v>
+        <v>159.4681262907357</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -635,25 +635,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6352490.512587539</v>
+        <v>2438174.532803317</v>
       </c>
       <c r="C9">
-        <v>86.21608638105322</v>
+        <v>207120.9900317253</v>
       </c>
       <c r="D9">
-        <v>93.88389918483716</v>
+        <v>29002.94097390444</v>
       </c>
       <c r="E9">
-        <v>16.58994151568492</v>
+        <v>3637.828952842845</v>
       </c>
       <c r="F9">
-        <v>4.147485378921229</v>
+        <v>909.4572382107112</v>
       </c>
       <c r="G9">
-        <v>114.6213260795921</v>
+        <v>33550.22716495767</v>
       </c>
       <c r="H9">
-        <v>0.8904055649840765</v>
+        <v>2801.128293688991</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -664,25 +664,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6352145.671413617</v>
+        <v>1821593.798410963</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>512.8441112129887</v>
+        <v>850609.1898334008</v>
       </c>
       <c r="E10">
-        <v>26.26758013553027</v>
+        <v>5314.20940450875</v>
       </c>
       <c r="F10">
-        <v>6.566895033882568</v>
+        <v>1328.552351127187</v>
       </c>
       <c r="G10">
-        <v>200.8374124607071</v>
+        <v>240671.2171966834</v>
       </c>
       <c r="H10">
-        <v>2.695865496298799</v>
+        <v>5103.423976479583</v>
       </c>
       <c r="I10">
         <v>8</v>
@@ -693,25 +693,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6351735.431366157</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>410.2400474597652</v>
+        <v>2168662.685807084</v>
       </c>
       <c r="D11">
-        <v>446.7559419774156</v>
+        <v>440993.9081771816</v>
       </c>
       <c r="E11">
-        <v>79.13811552398866</v>
+        <v>55351.32481258787</v>
       </c>
       <c r="F11">
-        <v>19.78452888099716</v>
+        <v>13837.83120314697</v>
       </c>
       <c r="G11">
-        <v>545.6785863824189</v>
+        <v>857251.9515890365</v>
       </c>
       <c r="H11">
-        <v>4.268481772023669</v>
+        <v>71614.5372174275</v>
       </c>
       <c r="I11">
         <v>9</v>
@@ -722,25 +722,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6350094.995789276</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2439.891529565515</v>
+        <v>2649111.867937323</v>
       </c>
       <c r="E12">
-        <v>125.1701449269209</v>
+        <v>23787.10565014157</v>
       </c>
       <c r="F12">
-        <v>31.29253623173022</v>
+        <v>5946.776412535393</v>
       </c>
       <c r="G12">
-        <v>955.9186338428408</v>
+        <v>2678845.75</v>
       </c>
       <c r="H12">
-        <v>12.85994377264816</v>
+        <v>77627.25862392764</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -751,25 +751,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6348143.880315402</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1951.115473873935</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>2125.472467716525</v>
+        <v>2307731.417963712</v>
       </c>
       <c r="E13">
-        <v>376.7053944061126</v>
+        <v>296891.4656290305</v>
       </c>
       <c r="F13">
-        <v>94.17634860152816</v>
+        <v>74222.86640725764</v>
       </c>
       <c r="G13">
-        <v>2596.354210724123</v>
+        <v>2678845.75</v>
       </c>
       <c r="H13">
-        <v>20.34014855062464</v>
+        <v>228606.4285343535</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -780,25 +780,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6340351.277937627</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>11596.00427620061</v>
+        <v>2010343.3010564</v>
       </c>
       <c r="E14">
-        <v>595.254228937092</v>
+        <v>534801.9591548798</v>
       </c>
       <c r="F14">
-        <v>148.813557234273</v>
+        <v>133700.4897887199</v>
       </c>
       <c r="G14">
-        <v>4547.469684598036</v>
+        <v>2678845.75</v>
       </c>
       <c r="H14">
-        <v>61.2146265909933</v>
+        <v>411797.5085492575</v>
       </c>
       <c r="I14">
         <v>12</v>
@@ -809,25 +809,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6331092.494662211</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>9258.783275416487</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>10101.67358914374</v>
+        <v>1751278.401222466</v>
       </c>
       <c r="E15">
-        <v>1790.718778582586</v>
+        <v>742053.8790220272</v>
       </c>
       <c r="F15">
-        <v>447.6796946456465</v>
+        <v>185513.4697555068</v>
       </c>
       <c r="G15">
-        <v>12340.07206237223</v>
+        <v>2678845.75</v>
       </c>
       <c r="H15">
-        <v>96.72881220227745</v>
+        <v>571381.4868469608</v>
       </c>
       <c r="I15">
         <v>13</v>
@@ -838,25 +838,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6294323.637750985</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>54843.62853917486</v>
+        <v>1525598.158770532</v>
       </c>
       <c r="E16">
-        <v>2819.266967871285</v>
+        <v>922598.0729835747</v>
       </c>
       <c r="F16">
-        <v>704.8167419678211</v>
+        <v>230649.5182458937</v>
       </c>
       <c r="G16">
-        <v>21598.85533778835</v>
+        <v>2678845.75</v>
       </c>
       <c r="H16">
-        <v>290.9918015196703</v>
+        <v>710400.5161973526</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -867,25 +867,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6250851.851892015</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>43471.78585896989</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>47776.14950384555</v>
+        <v>1329000.426442408</v>
       </c>
       <c r="E17">
-        <v>8473.250196134732</v>
+        <v>1079876.258846073</v>
       </c>
       <c r="F17">
-        <v>2118.312549033683</v>
+        <v>269969.0647115184</v>
       </c>
       <c r="G17">
-        <v>58367.71224901453</v>
+        <v>2678845.75</v>
       </c>
       <c r="H17">
-        <v>458.1308822790838</v>
+        <v>831504.7193114766</v>
       </c>
       <c r="I17">
         <v>15</v>
@@ -896,25 +896,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>6082755.416822709</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>253539.3903816155</v>
+        <v>1157737.457488481</v>
       </c>
       <c r="E18">
-        <v>13117.23423654065</v>
+        <v>1216886.634009215</v>
       </c>
       <c r="F18">
-        <v>3279.308559135163</v>
+        <v>304221.6585023038</v>
       </c>
       <c r="G18">
-        <v>101839.4981079847</v>
+        <v>2678845.75</v>
       </c>
       <c r="H18">
-        <v>1376.903156871894</v>
+        <v>937002.7081870958</v>
       </c>
       <c r="I18">
         <v>16</v>
@@ -925,25 +925,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>5888542.537240993</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>194212.8795817161</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>220866.7833006982</v>
+        <v>1008544.46229177</v>
       </c>
       <c r="E19">
-        <v>39255.31990127447</v>
+        <v>1336241.030166584</v>
       </c>
       <c r="F19">
-        <v>9813.829975318617</v>
+        <v>334060.257541646</v>
       </c>
       <c r="G19">
-        <v>269935.9331772905</v>
+        <v>2678845.75</v>
       </c>
       <c r="H19">
-        <v>2131.550563437856</v>
+        <v>1028905.59322827</v>
       </c>
       <c r="I19">
         <v>17</v>
@@ -954,25 +954,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>5220913.494530735</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1061070.149690331</v>
+        <v>878577.3716140791</v>
       </c>
       <c r="E20">
-        <v>56566.16462314687</v>
+        <v>1440214.702708737</v>
       </c>
       <c r="F20">
-        <v>14141.54115578672</v>
+        <v>360053.6756771842</v>
       </c>
       <c r="G20">
-        <v>464148.8127590064</v>
+        <v>2678845.75</v>
       </c>
       <c r="H20">
-        <v>6378.989483957101</v>
+        <v>1108965.321085728</v>
       </c>
       <c r="I20">
         <v>18</v>
@@ -983,25 +983,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>4523287.224598764</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>697626.2699319711</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>924334.2837803368</v>
+        <v>765358.620043659</v>
       </c>
       <c r="E21">
-        <v>165954.8573511423</v>
+        <v>1530789.703965073</v>
       </c>
       <c r="F21">
-        <v>41488.71433778557</v>
+        <v>382697.4259912682</v>
       </c>
       <c r="G21">
-        <v>1131777.855469265</v>
+        <v>2678845.75</v>
       </c>
       <c r="H21">
-        <v>9192.001751261367</v>
+        <v>1178708.072053106</v>
       </c>
       <c r="I21">
         <v>19</v>
@@ -1012,25 +1012,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2946637.994522575</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>3165296.067568534</v>
+        <v>666729.9161131128</v>
       </c>
       <c r="E22">
-        <v>192605.8303271122</v>
+        <v>1609692.66710951</v>
       </c>
       <c r="F22">
-        <v>48151.45758177806</v>
+        <v>402423.1667773774</v>
       </c>
       <c r="G22">
-        <v>1829404.125401235</v>
+        <v>2678845.75</v>
       </c>
       <c r="H22">
-        <v>26967.66431956062</v>
+        <v>1239463.353674323</v>
       </c>
       <c r="I22">
         <v>20</v>
@@ -1041,25 +1041,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1772083.004488584</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1174554.990033991</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>2757397.024525247</v>
+        <v>580811.0987432804</v>
       </c>
       <c r="E23">
-        <v>518925.0647617415</v>
+        <v>1678427.721005376</v>
       </c>
       <c r="F23">
-        <v>129731.2661904354</v>
+        <v>419606.9302513439</v>
       </c>
       <c r="G23">
-        <v>3406053.355477424</v>
+        <v>2678845.75</v>
       </c>
       <c r="H23">
-        <v>31298.44742815574</v>
+        <v>1292389.345174139</v>
       </c>
       <c r="I23">
         <v>21</v>
@@ -1070,25 +1070,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>704171.0970232752</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>5037337.070538723</v>
+        <v>505964.2956926289</v>
       </c>
       <c r="E24">
-        <v>488946.5459504012</v>
+        <v>1738305.163445897</v>
       </c>
       <c r="F24">
-        <v>122236.6364876003</v>
+        <v>434576.2908614743</v>
       </c>
       <c r="G24">
-        <v>4580608.345511416</v>
+        <v>2678845.75</v>
       </c>
       <c r="H24">
-        <v>84325.323023783</v>
+        <v>1338494.975853341</v>
       </c>
       <c r="I24">
         <v>22</v>
@@ -1099,25 +1099,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>257475.7390267292</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>446695.357996546</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>4388195.59160668</v>
+        <v>440762.7007639025</v>
       </c>
       <c r="E25">
-        <v>1008259.729096036</v>
+        <v>1790466.439388878</v>
       </c>
       <c r="F25">
-        <v>252064.9322740089</v>
+        <v>447616.6098472195</v>
       </c>
       <c r="G25">
-        <v>5648520.252976725</v>
+        <v>2678845.75</v>
       </c>
       <c r="H25">
-        <v>79453.81371694019</v>
+        <v>1378659.158329436</v>
       </c>
       <c r="I25">
         <v>23</v>
@@ -1128,25 +1128,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>91504.74641211731</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>4810823.033388617</v>
+        <v>383963.3745672614</v>
       </c>
       <c r="E26">
-        <v>1160290.856159413</v>
+        <v>1835905.900346191</v>
       </c>
       <c r="F26">
-        <v>290072.7140398532</v>
+        <v>458976.4750865478</v>
       </c>
       <c r="G26">
-        <v>6095215.610973271</v>
+        <v>2678845.75</v>
       </c>
       <c r="H26">
-        <v>163842.2059781058</v>
+        <v>1413647.543266567</v>
       </c>
       <c r="I26">
         <v>24</v>
@@ -1157,25 +1157,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>36068.31892645982</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>55436.42748565751</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>4190871.51236796</v>
+        <v>334483.5503402767</v>
       </c>
       <c r="E27">
-        <v>1656252.072975939</v>
+        <v>1875489.759727779</v>
       </c>
       <c r="F27">
-        <v>414063.0182439848</v>
+        <v>468872.4399319447</v>
       </c>
       <c r="G27">
-        <v>6261186.603587883</v>
+        <v>2678845.75</v>
       </c>
       <c r="H27">
-        <v>188547.2641259046</v>
+        <v>1444127.11499039</v>
       </c>
       <c r="I27">
         <v>25</v>
@@ -1186,25 +1186,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>16506.1961687579</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>3806528.915536088</v>
+        <v>291379.9931421266</v>
       </c>
       <c r="E28">
-        <v>2023724.990636123</v>
+        <v>1909972.605486299</v>
       </c>
       <c r="F28">
-        <v>505931.2476590307</v>
+        <v>477493.1513715747</v>
       </c>
       <c r="G28">
-        <v>6316623.03107354</v>
+        <v>2678845.75</v>
       </c>
       <c r="H28">
-        <v>269140.9618585901</v>
+        <v>1470678.90622445</v>
       </c>
       <c r="I28">
         <v>26</v>
@@ -1215,25 +1215,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>8593.79375029153</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>7912.402418466364</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>3315996.760306615</v>
+        <v>253831.0189458732</v>
       </c>
       <c r="E29">
-        <v>2416150.714819701</v>
+        <v>1940011.784843301</v>
       </c>
       <c r="F29">
-        <v>604037.6787049253</v>
+        <v>485002.9462108253</v>
       </c>
       <c r="G29">
-        <v>6336185.153831242</v>
+        <v>2678845.75</v>
       </c>
       <c r="H29">
-        <v>328855.31097837</v>
+        <v>1493809.074329342</v>
       </c>
       <c r="I29">
         <v>27</v>
@@ -1244,25 +1244,25 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4983.131125689103</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>2915361.866201557</v>
+        <v>221120.8308583943</v>
       </c>
       <c r="E30">
-        <v>2745877.082138203</v>
+        <v>1966179.935313284</v>
       </c>
       <c r="F30">
-        <v>686469.2705345507</v>
+        <v>491544.9838283211</v>
       </c>
       <c r="G30">
-        <v>6344097.556249708</v>
+        <v>2678845.75</v>
       </c>
       <c r="H30">
-        <v>392624.4911582015</v>
+        <v>1513958.550191229</v>
       </c>
       <c r="I30">
         <v>28</v>
@@ -1273,25 +1273,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3153.653865394874</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>1829.477260294228</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>2539670.843951627</v>
+        <v>192625.8738689965</v>
       </c>
       <c r="E31">
-        <v>3046429.899938147</v>
+        <v>1988975.900904803</v>
       </c>
       <c r="F31">
-        <v>761607.4749845368</v>
+        <v>497243.9752262008</v>
       </c>
       <c r="G31">
-        <v>6347708.21887431</v>
+        <v>2678845.75</v>
       </c>
       <c r="H31">
-        <v>446205.0258474579</v>
+        <v>1531511.443696698</v>
       </c>
       <c r="I31">
         <v>29</v>
@@ -1302,25 +1302,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>2142.914612950391</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2219336.830054891</v>
+        <v>167802.9480069944</v>
       </c>
       <c r="E32">
-        <v>3304969.284265726</v>
+        <v>2008834.241594405</v>
       </c>
       <c r="F32">
-        <v>826242.3210664315</v>
+        <v>502208.5603986012</v>
       </c>
       <c r="G32">
-        <v>6349537.696134605</v>
+        <v>2678845.75</v>
       </c>
       <c r="H32">
-        <v>495044.8587399489</v>
+        <v>1546802.366027692</v>
       </c>
       <c r="I32">
         <v>30</v>
@@ -1331,25 +1331,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1544.006331447481</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>598.90828150291</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>1933339.770113038</v>
+        <v>146178.853309125</v>
       </c>
       <c r="E33">
-        <v>3533766.93221921</v>
+        <v>2026133.5173527</v>
       </c>
       <c r="F33">
-        <v>883441.7330548024</v>
+        <v>506533.3793381751</v>
       </c>
       <c r="G33">
-        <v>6350548.435387049</v>
+        <v>2678845.75</v>
       </c>
       <c r="H33">
-        <v>537057.5086931805</v>
+        <v>1560122.808361579</v>
       </c>
       <c r="I33">
         <v>31</v>
@@ -1360,25 +1360,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1167.720217284553</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>1686656.308178567</v>
+        <v>127341.3691985913</v>
       </c>
       <c r="E34">
-        <v>3731893.857283318</v>
+        <v>2041203.504641127</v>
       </c>
       <c r="F34">
-        <v>932973.4643208296</v>
+        <v>510300.8761602818</v>
       </c>
       <c r="G34">
-        <v>6351147.343668552</v>
+        <v>2678845.75</v>
       </c>
       <c r="H34">
-        <v>574237.1264856216</v>
+        <v>1571726.698573668</v>
       </c>
       <c r="I34">
         <v>32</v>
@@ -1389,25 +1389,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>919.6939793127506</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>248.0262379718025</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>1469303.656368828</v>
+        <v>110931.3963154456</v>
       </c>
       <c r="E35">
-        <v>3905775.97873111</v>
+        <v>2054331.482947643</v>
       </c>
       <c r="F35">
-        <v>976443.9946827774</v>
+        <v>513582.8707369108</v>
       </c>
       <c r="G35">
-        <v>6351523.629782715</v>
+        <v>2678845.75</v>
       </c>
       <c r="H35">
-        <v>606432.7518085393</v>
+        <v>1581835.241869686</v>
       </c>
       <c r="I35">
         <v>33</v>
@@ -1418,25 +1418,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>749.4253955970053</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>1281034.757838621</v>
+        <v>96636.11099785942</v>
       </c>
       <c r="E36">
-        <v>4056725.733412626</v>
+        <v>2065767.711201712</v>
       </c>
       <c r="F36">
-        <v>1014181.433353156</v>
+        <v>516441.9278004281</v>
       </c>
       <c r="G36">
-        <v>6351771.656020687</v>
+        <v>2678845.75</v>
       </c>
       <c r="H36">
-        <v>634688.5965438053</v>
+        <v>1590641.137625318</v>
       </c>
       <c r="I36">
         <v>34</v>
@@ -1447,25 +1447,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>628.5267178840736</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>120.8986777129315</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>1115952.932734989</v>
+        <v>84183.00191800926</v>
       </c>
       <c r="E37">
-        <v>4188791.19349553</v>
+        <v>2075730.198465592</v>
       </c>
       <c r="F37">
-        <v>1047197.798373883</v>
+        <v>518932.5496163981</v>
       </c>
       <c r="G37">
-        <v>6351941.924604403</v>
+        <v>2678845.75</v>
       </c>
       <c r="H37">
-        <v>659217.9316795517</v>
+        <v>1598312.252818506</v>
       </c>
       <c r="I37">
         <v>35</v>
@@ -1476,25 +1476,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>540.1644057550124</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>972688.5145767028</v>
+        <v>73334.67519284307</v>
       </c>
       <c r="E38">
-        <v>4303570.136814034</v>
+        <v>2084408.859845726</v>
       </c>
       <c r="F38">
-        <v>1075892.534203508</v>
+        <v>521102.2149614314</v>
       </c>
       <c r="G38">
-        <v>6352062.823282115</v>
+        <v>2678845.75</v>
       </c>
       <c r="H38">
-        <v>680678.5689430237</v>
+        <v>1604994.822081208</v>
       </c>
       <c r="I38">
         <v>36</v>
@@ -1505,25 +1505,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>473.9988473151489</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>66.1655584398635</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>847342.0364572614</v>
+        <v>63884.32893944216</v>
       </c>
       <c r="E39">
-        <v>4403847.319309587</v>
+        <v>2091969.136848446</v>
       </c>
       <c r="F39">
-        <v>1100961.829827397</v>
+        <v>522992.2842121116</v>
       </c>
       <c r="G39">
-        <v>6352151.185594245</v>
+        <v>2678845.75</v>
       </c>
       <c r="H39">
-        <v>699330.1472322805</v>
+        <v>1610816.235373304</v>
       </c>
       <c r="I39">
         <v>37</v>
@@ -1534,25 +1534,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>423.4058080308445</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>738454.3997259369</v>
+        <v>55651.81100633201</v>
       </c>
       <c r="E40">
-        <v>4491050.835572827</v>
+        <v>2098555.151194935</v>
       </c>
       <c r="F40">
-        <v>1122762.708893207</v>
+        <v>524638.7877987337</v>
       </c>
       <c r="G40">
-        <v>6352217.351152685</v>
+        <v>2678845.75</v>
       </c>
       <c r="H40">
-        <v>715625.1893878079</v>
+        <v>1615887.4664201</v>
       </c>
       <c r="I40">
         <v>38</v>
@@ -1563,25 +1563,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>384.0315189827995</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>39.3742890480448</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>643292.7350508542</v>
+        <v>48480.18472919</v>
       </c>
       <c r="E41">
-        <v>4567180.167312892</v>
+        <v>2104292.452216648</v>
       </c>
       <c r="F41">
-        <v>1141795.041828223</v>
+        <v>526073.1130541619</v>
       </c>
       <c r="G41">
-        <v>6352267.944191969</v>
+        <v>2678845.75</v>
       </c>
       <c r="H41">
-        <v>729795.7607805844</v>
+        <v>1620305.188206819</v>
       </c>
       <c r="I41">
         <v>39</v>
@@ -1592,25 +1592,25 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>352.913943508613</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>560579.8921810609</v>
+        <v>42232.73724387821</v>
       </c>
       <c r="E42">
-        <v>4633406.835100344</v>
+        <v>2109290.410204898</v>
       </c>
       <c r="F42">
-        <v>1158351.708775086</v>
+        <v>527322.6025512244</v>
       </c>
       <c r="G42">
-        <v>6352307.318481017</v>
+        <v>2678845.75</v>
       </c>
       <c r="H42">
-        <v>742166.777188345</v>
+        <v>1624153.615857771</v>
       </c>
       <c r="I42">
         <v>40</v>
@@ -1621,25 +1621,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>328.0002243302051</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>24.91371917840791</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>488340.2037952563</v>
+        <v>36790.3733262086</v>
       </c>
       <c r="E43">
-        <v>4691198.585808988</v>
+        <v>2113644.301339033</v>
       </c>
       <c r="F43">
-        <v>1172799.646452247</v>
+        <v>528411.0753347583</v>
       </c>
       <c r="G43">
-        <v>6352338.436056491</v>
+        <v>2678845.75</v>
       </c>
       <c r="H43">
-        <v>752928.610703806</v>
+        <v>1627506.112031056</v>
       </c>
       <c r="I43">
         <v>41</v>
@@ -1650,25 +1650,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>307.8253067743839</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>425528.9995412677</v>
+        <v>32049.3450771534</v>
       </c>
       <c r="E44">
-        <v>4741483.620121566</v>
+        <v>2117437.123938277</v>
       </c>
       <c r="F44">
-        <v>1185370.905030391</v>
+        <v>529359.2809845693</v>
       </c>
       <c r="G44">
-        <v>6352363.349775669</v>
+        <v>2678845.75</v>
       </c>
       <c r="H44">
-        <v>762319.7701939605</v>
+        <v>1630426.585432474</v>
       </c>
       <c r="I44">
         <v>42</v>
@@ -1679,25 +1679,25 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>291.3297980070408</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>16.49550876734314</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>370692.7794863827</v>
+        <v>27919.27417444095</v>
       </c>
       <c r="E45">
-        <v>4785352.596165474</v>
+        <v>2120741.180660447</v>
       </c>
       <c r="F45">
-        <v>1196338.149041368</v>
+        <v>530185.2951651118</v>
       </c>
       <c r="G45">
-        <v>6352383.524693226</v>
+        <v>2678845.75</v>
       </c>
       <c r="H45">
-        <v>770491.0882697544</v>
+        <v>1632970.709108544</v>
       </c>
       <c r="I45">
         <v>43</v>
@@ -1708,25 +1708,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>277.7277472687484</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>323002.8979296609</v>
+        <v>24321.42898867745</v>
       </c>
       <c r="E46">
-        <v>4823528.579458456</v>
+        <v>2123619.456809058</v>
       </c>
       <c r="F46">
-        <v>1205882.144864614</v>
+        <v>530904.8642022645</v>
       </c>
       <c r="G46">
-        <v>6352400.020201992</v>
+        <v>2678845.75</v>
       </c>
       <c r="H46">
-        <v>777619.7968768895</v>
+        <v>1635186.981742975</v>
       </c>
       <c r="I46">
         <v>44</v>
@@ -1737,25 +1737,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>266.4308827102923</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>11.29686455845612</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>281378.8064850573</v>
+        <v>21187.22372062254</v>
       </c>
       <c r="E47">
-        <v>4856827.852614139</v>
+        <v>2126126.821023502</v>
       </c>
       <c r="F47">
-        <v>1214206.963153535</v>
+        <v>531531.7052558755</v>
       </c>
       <c r="G47">
-        <v>6352413.622252731</v>
+        <v>2678845.75</v>
       </c>
       <c r="H47">
-        <v>783823.3941619991</v>
+        <v>1637117.652188096</v>
       </c>
       <c r="I47">
         <v>45</v>
@@ -1766,25 +1766,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>256.9886500856697</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>245173.7499356657</v>
+        <v>18456.91094864079</v>
       </c>
       <c r="E48">
-        <v>4885808.489131398</v>
+        <v>2128311.071241087</v>
       </c>
       <c r="F48">
-        <v>1221452.12228285</v>
+        <v>532077.7678102718</v>
       </c>
       <c r="G48">
-        <v>6352424.91911729</v>
+        <v>2678845.75</v>
       </c>
       <c r="H48">
-        <v>789234.5260497977</v>
+        <v>1638799.524855637</v>
       </c>
       <c r="I48">
         <v>46</v>
@@ -1795,25 +1795,25 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>249.0541394902625</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>7.934510595407194</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>213579.1894764563</v>
+        <v>16078.44266233325</v>
       </c>
       <c r="E49">
-        <v>4911084.137498766</v>
+        <v>2130213.845870133</v>
       </c>
       <c r="F49">
-        <v>1227771.034374692</v>
+        <v>532553.4614675334</v>
       </c>
       <c r="G49">
-        <v>6352434.361349914</v>
+        <v>2678845.75</v>
       </c>
       <c r="H49">
-        <v>793943.8794838523</v>
+        <v>1640264.661320003</v>
       </c>
       <c r="I49">
         <v>47</v>
@@ -1824,25 +1824,25 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>242.3545705873175</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>186095.0326961245</v>
+        <v>14006.47807020901</v>
       </c>
       <c r="E50">
-        <v>4933083.17018663</v>
+        <v>2131871.417543833</v>
       </c>
       <c r="F50">
-        <v>1233270.792546658</v>
+        <v>532967.8543859583</v>
       </c>
       <c r="G50">
-        <v>6352442.295860509</v>
+        <v>2678845.75</v>
       </c>
       <c r="H50">
-        <v>798051.1723435496</v>
+        <v>1641540.991508751</v>
       </c>
       <c r="I50">
         <v>48</v>
@@ -1853,25 +1853,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>236.6749643539687</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>5.679606233348904</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>162113.7102127057</v>
+        <v>12201.51926721346</v>
       </c>
       <c r="E51">
-        <v>4952268.228173366</v>
+        <v>2133315.384586229</v>
       </c>
       <c r="F51">
-        <v>1238067.057043341</v>
+        <v>533328.8461465572</v>
       </c>
       <c r="G51">
-        <v>6352448.995429412</v>
+        <v>2678845.75</v>
       </c>
       <c r="H51">
-        <v>801626.0151553275</v>
+        <v>1642652.846131397</v>
       </c>
       <c r="I51">
         <v>49</v>
@@ -1882,25 +1882,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>231.8425633336233</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>141250.7651570821</v>
+        <v>10629.15828532473</v>
       </c>
       <c r="E52">
-        <v>4968966.993823667</v>
+        <v>2134573.27337174</v>
       </c>
       <c r="F52">
-        <v>1242241.748455917</v>
+        <v>533643.3183429351</v>
       </c>
       <c r="G52">
-        <v>6352454.675035645</v>
+        <v>2678845.75</v>
       </c>
       <c r="H52">
-        <v>804743.587078172</v>
+        <v>1643621.42049624</v>
       </c>
       <c r="I52">
         <v>50</v>

</xml_diff>